<commit_message>
updated arduino code to fix communication bug
</commit_message>
<xml_diff>
--- a/CAD/hardware_bom.xlsx
+++ b/CAD/hardware_bom.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25823"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28880" windowHeight="19660" tabRatio="500"/>
+    <workbookView xWindow="16440" yWindow="-20" windowWidth="16440" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -115,9 +115,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>952-2018-ND</t>
-  </si>
-  <si>
     <t>3.5mm Audio Cable</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>5/16 nuts</t>
+  </si>
+  <si>
+    <t>952-2189-ND</t>
   </si>
   <si>
     <r>
@@ -160,21 +160,15 @@
         <color indexed="23"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>$127.67 + ~ $10 for fasteners</t>
+      <t>$128.79 + ~ $10 for fasteners</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -305,7 +299,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -331,13 +325,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -660,14 +655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -848,25 +843,25 @@
       <c r="C12" s="3">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
+      <c r="D12" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E12" s="3">
-        <v>1.1200000000000001</v>
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3">
         <v>5.99</v>
@@ -874,7 +869,7 @@
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -883,7 +878,7 @@
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -894,7 +889,7 @@
     </row>
     <row r="16" spans="1:5" ht="25" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3">
@@ -905,7 +900,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -916,7 +911,7 @@
     </row>
     <row r="18" spans="1:5" ht="25" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -927,7 +922,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -938,7 +933,7 @@
     </row>
     <row r="20" spans="1:5" ht="25" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -949,7 +944,7 @@
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -984,12 +979,12 @@
     <hyperlink ref="D9" r:id="rId5"/>
     <hyperlink ref="D10" r:id="rId6"/>
     <hyperlink ref="D11" r:id="rId7"/>
-    <hyperlink ref="D12" r:id="rId8"/>
-    <hyperlink ref="D13" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>